<commit_message>
check data validation and connect to sql server
</commit_message>
<xml_diff>
--- a/HPTN083-XN-1.3b.xlsx
+++ b/HPTN083-XN-1.3b.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unchnsrv01\11 SHARING\HPTN 083 Database\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nguyen Huy Dinh\Documents\20182\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F954B153-5B36-4AD9-867E-426D93F16027}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EC39AC8-19C8-4188-8B1B-3776918AD27E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XN-1b" sheetId="4" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Urea</t>
   </si>
@@ -100,54 +103,7 @@
     <t>Năm sinh:</t>
   </si>
   <si>
-    <t>Giới tính: Nam</t>
-  </si>
-  <si>
     <t>Loại mẫu thu thập</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>□</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Máu toàn phần            Ống Lithium-Heparine 4ml x 1 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>□</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Máu toàn phần          Ống Flouride 2ml x 1 </t>
-    </r>
   </si>
   <si>
     <t>Loại mẫu phân tích trên máy</t>
@@ -218,6 +174,18 @@
   <si>
     <t xml:space="preserve">                        Ngày:</t>
   </si>
+  <si>
+    <t xml:space="preserve">Máu toàn phần            Ống Lithium-Heparine 4ml x 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Máu toàn phần          Ống Flouride 2ml x 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giới tính: </t>
+  </si>
+  <si>
+    <t>Nguyễn Huy Định</t>
+  </si>
 </sst>
 </file>
 
@@ -241,13 +209,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -289,6 +250,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -458,22 +425,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -507,13 +474,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,13 +496,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -567,6 +534,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX8.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX9.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1179,7 +1206,906 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="cmdBtn" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="lithiumCb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="flourideCb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>1695450</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>447675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="idTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1457325</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>952500</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>447675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="tuanTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>704850</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>1609725</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>409575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="namsinhTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>714375</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>666750</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>400050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="gioitinhTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1266825</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>857250</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>447675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1037" name="ngayyeucauTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1037"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>981075</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>762000</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>438150</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1038" name="ngaylaymauTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1038"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>704850</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>323850</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>447675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="giolaymauTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1323975</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>704850</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>342900</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1041" name="ngaycokqTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1041"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>361950</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="ngaynhanmauTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>971550</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>352425</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1043" name="gionhanmauTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1043"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1045" name="ngaysaottTb" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1045"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1390650</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>800100</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1053" name="Button 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1053"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Button 2</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="XN-1b"/>
+      <sheetName val="HPTN083-XN-1.3b (1)"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="Button2_Click"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1502,24 +2428,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD29"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
@@ -1528,7 +2455,7 @@
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>22</v>
       </c>
@@ -1537,7 +2464,7 @@
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>13</v>
       </c>
@@ -1547,7 +2474,7 @@
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
@@ -1557,32 +2484,32 @@
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="28"/>
       <c r="D5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>16</v>
       </c>
@@ -1593,13 +2520,13 @@
         <v>18</v>
       </c>
       <c r="D8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
@@ -1608,13 +2535,13 @@
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>1</v>
       </c>
@@ -1625,7 +2552,7 @@
       <c r="D10" s="36"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>2</v>
       </c>
@@ -1636,7 +2563,7 @@
       <c r="D11" s="36"/>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +2574,7 @@
       <c r="D12" s="36"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>4</v>
       </c>
@@ -1658,7 +2585,7 @@
       <c r="D13" s="36"/>
       <c r="E13" s="30"/>
     </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>6</v>
       </c>
@@ -1669,7 +2596,7 @@
       <c r="D14" s="36"/>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>7</v>
       </c>
@@ -1680,14 +2607,14 @@
       <c r="D15" s="36"/>
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:5" ht="3" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="10"/>
       <c r="C16" s="9"/>
       <c r="D16" s="36"/>
       <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>23</v>
       </c>
@@ -1698,7 +2625,7 @@
       <c r="D17" s="36"/>
       <c r="E17" s="30"/>
     </row>
-    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +2636,7 @@
       <c r="D18" s="36"/>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>9</v>
       </c>
@@ -1720,7 +2647,7 @@
       <c r="D19" s="36"/>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>11</v>
       </c>
@@ -1731,14 +2658,14 @@
       <c r="D20" s="36"/>
       <c r="E20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="10"/>
       <c r="C21" s="9"/>
       <c r="D21" s="37"/>
       <c r="E21" s="31"/>
     </row>
-    <row r="22" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>5</v>
       </c>
@@ -1747,60 +2674,63 @@
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="21" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="D31" s="27" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1822,5 +2752,380 @@
     <oddFooter>&amp;R&amp;9Phòng khám Đa khoa Yên Hòa</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1045" r:id="rId4" name="ngaysaottTb">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1047750</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1019175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1045" r:id="rId4" name="ngaysaottTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1043" r:id="rId6" name="gionhanmauTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>971550</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>542925</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>352425</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1043" r:id="rId6" name="gionhanmauTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1042" r:id="rId8" name="ngaynhanmauTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>361950</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1042" r:id="rId8" name="ngaynhanmauTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1041" r:id="rId10" name="ngaycokqTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1323975</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>704850</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>342900</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1041" r:id="rId10" name="ngaycokqTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1039" r:id="rId12" name="giolaymauTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>704850</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>323850</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>447675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1039" r:id="rId12" name="giolaymauTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId14" name="ngaylaymauTb">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>981075</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>762000</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>438150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId14" name="ngaylaymauTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1037" r:id="rId16" name="ngayyeucauTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1266825</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>447675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1037" r:id="rId16" name="ngayyeucauTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId18" name="gioitinhTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>714375</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>666750</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>400050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId18" name="gioitinhTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1034" r:id="rId20" name="namsinhTb">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>704850</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>1609725</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>409575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1034" r:id="rId20" name="namsinhTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1032" r:id="rId22" name="tuanTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1457325</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>952500</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>447675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1032" r:id="rId22" name="tuanTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1031" r:id="rId24" name="idTb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>1695450</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>504825</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>447675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1031" r:id="rId24" name="idTb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId26" name="flourideCb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>285750</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId26" name="flourideCb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId28" name="lithiumCb">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>200025</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId28" name="lithiumCb"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId30" name="cmdBtn">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId30" name="cmdBtn"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1053" r:id="rId32" name="Button 29">
+          <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Button2_Click">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1390650</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>800100</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
</xml_diff>